<commit_message>
Feat: Added basline tests
</commit_message>
<xml_diff>
--- a/Baseline_For_StackedAE/BaseLine_Tests.xlsx
+++ b/Baseline_For_StackedAE/BaseLine_Tests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D0DC80-FB8D-47CD-A644-7AD872E3CC3A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FD4629-439B-4EA7-B7DA-A61F5D91A40F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,26 +52,27 @@
     <t>Gamma = 0.1  Kernel = polynomial</t>
   </si>
   <si>
-    <t>Clusters = 10
-Feed into SVM for finding accuracy: 
-Train data = KMeans of mnst train data Train label = MNIST train labels 
-Test data = Kmeans of mnist test data
-Test labels = MNIST test labels</t>
-  </si>
-  <si>
     <t>TensorFlow 
 3 Hidden layers: 500 &gt;&gt;200 &gt;&gt; 100 
 Activations: Sigmoid</t>
   </si>
   <si>
     <t>Solver = 'lbfgs'</t>
+  </si>
+  <si>
+    <t>Clusters = 10
+Feed into SVM for finding accuracy: 
+Train data = KMeans of mnst train data
+Train label = MNIST train labels 
+Test data = Kmeans of mnist test data
+Test labels = MNIST test labels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,8 +81,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -286,103 +294,107 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,217 +676,238 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I17"/>
+  <dimension ref="B1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:G6"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="11.88671875" style="1" customWidth="1"/>
+    <col min="4" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="5.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="51.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+    <row r="1" spans="2:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="22"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="7"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11">
+      <c r="D4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12">
         <v>0.87580000000000002</v>
       </c>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I4" s="13"/>
+      <c r="L4" s="34"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="L6" s="34"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="14">
+        <v>0.84140000000000004</v>
+      </c>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" spans="2:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="13">
-        <v>0.84140000000000004</v>
-      </c>
-      <c r="I7" s="14"/>
-    </row>
-    <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18">
-        <v>0.87749999999999995</v>
-      </c>
-      <c r="I8" s="19"/>
-    </row>
-    <row r="9" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="22"/>
-    </row>
-    <row r="12" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
-        <v>6</v>
-      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="26">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="24"/>
       <c r="C12" s="25"/>
-      <c r="D12" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="26">
-        <v>0.56000000000000005</v>
-      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="26"/>
       <c r="I12" s="27"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="24"/>
       <c r="C13" s="25"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="26"/>
       <c r="I13" s="27"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="24"/>
       <c r="C14" s="25"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
       <c r="H14" s="26"/>
       <c r="I14" s="27"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="24"/>
       <c r="C15" s="25"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
       <c r="H15" s="26"/>
       <c r="I15" s="27"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="27"/>
-    </row>
-    <row r="17" spans="2:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="32"/>
+    <row r="16" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
+    <mergeCell ref="D11:G16"/>
+    <mergeCell ref="B11:C16"/>
+    <mergeCell ref="H11:I16"/>
+    <mergeCell ref="D4:G6"/>
+    <mergeCell ref="B4:C6"/>
+    <mergeCell ref="H4:I6"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D7:G7"/>
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:C3"/>
@@ -882,20 +915,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D12:G17"/>
-    <mergeCell ref="B12:C17"/>
-    <mergeCell ref="H12:I17"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="D4:G6"/>
-    <mergeCell ref="B4:C6"/>
-    <mergeCell ref="H4:I6"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>